<commit_message>
Added data driven approach in framework with POJO bean class and TestNg dataprovider.
</commit_message>
<xml_diff>
--- a/AutomateIt/resources/testData/orangeHRMData.xlsx
+++ b/AutomateIt/resources/testData/orangeHRMData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prateek.sethi/git/AutomateIt/AutomateIt/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB57D492-65E0-CF40-B27B-81142B0E9DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19DD49E-28DF-C64F-B041-482402108704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38140" yWindow="1380" windowWidth="28040" windowHeight="17440" xr2:uid="{D490E847-767A-734B-96BD-DFF9779B5DB7}"/>
+    <workbookView xWindow="38020" yWindow="1320" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{D490E847-767A-734B-96BD-DFF9779B5DB7}"/>
   </bookViews>
   <sheets>
-    <sheet name="AdminUserBean" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginUserBean" sheetId="2" r:id="rId1"/>
+    <sheet name="AdminUserBean" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>employeeName</t>
   </si>
@@ -91,6 +92,21 @@
   </si>
   <si>
     <t>searchUserDataProvider</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>validUserLoginDataProvider</t>
+  </si>
+  <si>
+    <t>Linda.Anderson</t>
+  </si>
+  <si>
+    <t>Linda Jane Anderson</t>
   </si>
 </sst>
 </file>
@@ -461,18 +477,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DFE5EEC-5292-E34C-9CE8-1286A514616E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D24F022-EA86-2240-8C1F-BE8A672B3C69}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -559,6 +615,23 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -568,7 +641,6 @@
     <hyperlink ref="G2" r:id="rId2" xr:uid="{EDE44F2B-F26A-384C-B8A6-BA05B8E53778}"/>
     <hyperlink ref="G3" r:id="rId3" xr:uid="{A391FABF-8B0D-CE4E-8926-5F738967BD76}"/>
     <hyperlink ref="F3" r:id="rId4" xr:uid="{6A788AC2-3756-434A-ABF5-C62395600416}"/>
-    <hyperlink ref="D4" r:id="rId5" display="https://opensource-demo.orangehrmlive.com/index.php/admin/saveSystemUser?userId=21" xr:uid="{C58DB519-C4CC-FE45-88E0-98F81AA4CAB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>